<commit_message>
all up and running cleaned code
Signed-off-by: Pritom <naitiq@yahoo.com>
</commit_message>
<xml_diff>
--- a/Performance Evaluation.xlsx
+++ b/Performance Evaluation.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ollie\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pritom\PycharmProjects\SearchFlow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9C8D64-D7FD-4725-B75C-308DEE16B23B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CCBA7BF7-8A6F-4DC4-A058-2421D7042269}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -189,7 +188,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -256,17 +255,17 @@
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,23 +579,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86011E01-5F66-47FC-8941-5EE96FC47613}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.7265625" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" customWidth="1"/>
-    <col min="5" max="5" width="20.7265625" customWidth="1"/>
-    <col min="6" max="6" width="24.36328125" customWidth="1"/>
-    <col min="7" max="7" width="26.81640625" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" customWidth="1"/>
+    <col min="7" max="7" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -621,8 +622,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
@@ -647,25 +648,25 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
       <c r="H3" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
@@ -687,11 +688,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
@@ -713,11 +714,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C6" t="s">
@@ -739,11 +740,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
@@ -765,11 +766,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C8" t="s">
@@ -791,25 +792,25 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
       <c r="H9" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="s">
@@ -831,11 +832,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C11" t="s">
@@ -857,11 +858,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C12" t="s">
@@ -883,11 +884,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C13" t="s">
@@ -909,11 +910,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C14" t="s">
@@ -935,190 +936,190 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
       <c r="H15" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <f>ABS(ROW(B4)-3-IFERROR(MATCH(B4,B$10:B$14,0),ROW(B4)+2))</f>
         <v>1</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <f t="shared" ref="C16:G16" si="0">ABS(ROW(C4)-3-IFERROR(MATCH(C4,C$10:C$14,0),ROW(C4)+2))</f>
         <v>0</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="4">
         <f t="shared" ref="B17:G17" si="1">ABS(ROW(B5)-3-IFERROR(MATCH(B5,B$10:B$14,0),ROW(B5)+2))</f>
         <v>1</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="4">
         <f t="shared" ref="B18:G18" si="2">ABS(ROW(B6)-3-IFERROR(MATCH(B6,B$10:B$14,0),ROW(B6)+2))</f>
         <v>0</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="4">
         <f t="shared" ref="B19:G19" si="3">ABS(ROW(B7)-3-IFERROR(MATCH(B7,B$10:B$14,0),ROW(B7)+2))</f>
         <v>0</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="4">
         <f t="shared" ref="B20:G20" si="4">ABS(ROW(B8)-3-IFERROR(MATCH(B8,B$10:B$14,0),ROW(B8)+2))</f>
         <v>0</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="4">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="6">
         <f>EXP(-SUM(B16:B20)/5)</f>
         <v>0.67032004603563933</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="6">
         <f t="shared" ref="C21:G21" si="5">EXP(-SUM(C16:C20)/5)</f>
         <v>0.36787944117144233</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="6">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="6">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="6">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="6">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>

</xml_diff>